<commit_message>
template 2 todays sate
</commit_message>
<xml_diff>
--- a/webscrapping school/msaces/excel/2025-07-28.xlsx
+++ b/webscrapping school/msaces/excel/2025-07-28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,11 @@
           <t>CapitalSocial</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Forma Jurídica</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -620,6 +625,11 @@
           <t>€ 2.500,00</t>
         </is>
       </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Sociedade por Quotas</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -711,6 +721,11 @@
           <t>€ 2.000,00</t>
         </is>
       </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Sociedade por Quotas</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -802,6 +817,11 @@
           <t>€ 50.184,00</t>
         </is>
       </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Sociedade por Quotas</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -893,6 +913,11 @@
           <t>€ 1.000,00</t>
         </is>
       </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Sociedade por Quotas</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -984,6 +1009,11 @@
           <t>€ 47.000.000,00</t>
         </is>
       </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Sociedade Anónima</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1075,6 +1105,11 @@
           <t>€ 5.000,00</t>
         </is>
       </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Sociedade por Quotas</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1166,6 +1201,11 @@
           <t>Não disponível</t>
         </is>
       </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Sociedade por Quotas</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1257,6 +1297,11 @@
           <t>€ 50.000,00</t>
         </is>
       </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Sociedade Anónima</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1348,6 +1393,11 @@
           <t>€ 35.000,00</t>
         </is>
       </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Sociedade por Quotas</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1443,6 +1493,11 @@
           <t>€ 2.000,00</t>
         </is>
       </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Sociedade Unipessoal</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1534,6 +1589,11 @@
           <t>€ 5.000,00</t>
         </is>
       </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>Sociedade por Quotas</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1625,6 +1685,11 @@
           <t>€ 25.000,00</t>
         </is>
       </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>Sociedade Unipessoal</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1716,6 +1781,11 @@
           <t>€ 2.000,00</t>
         </is>
       </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Sociedade por Quotas</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1811,6 +1881,11 @@
           <t>€ 200.000,00</t>
         </is>
       </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>Sociedade por Quotas</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1902,6 +1977,11 @@
           <t>€ 10.000,00</t>
         </is>
       </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>Sociedade Unipessoal</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1989,6 +2069,11 @@
       <c r="S17" t="inlineStr">
         <is>
           <t>€ 20.000,00</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>Sociedade Unipessoal</t>
         </is>
       </c>
     </row>

</xml_diff>